<commit_message>
Se agraga modulo Resico
</commit_message>
<xml_diff>
--- a/Calculo RESICO.xlsx
+++ b/Calculo RESICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dtax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3642B55-9ABE-4BC6-ABD2-D1BD351D04A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA26AC85-2398-48E0-9E89-D279BA5E9CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D021B31C-5EFD-4BFB-8E44-7D77FAE79C49}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>f11-f12</t>
   </si>
   <si>
-    <t>f26-f28</t>
-  </si>
-  <si>
     <t>IVA Retenido</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>I1+I2</t>
   </si>
   <si>
-    <t>F26-I6</t>
-  </si>
-  <si>
     <t>operaciones</t>
   </si>
   <si>
@@ -445,6 +439,12 @@
   </si>
   <si>
     <t>V19+V20</t>
+  </si>
+  <si>
+    <t>I21-I22-I23</t>
+  </si>
+  <si>
+    <t>f26--F27-f28</t>
   </si>
 </sst>
 </file>
@@ -836,6 +836,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,10 +848,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED7E331-9773-4746-BEB0-64B639BA38E8}">
   <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,15 +1186,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1203,7 +1203,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="32"/>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="27"/>
@@ -1254,18 +1254,18 @@
         <v>27</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="27"/>
@@ -1281,24 +1281,24 @@
         <v>26</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="str">
@@ -1317,20 +1317,20 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>I4</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="43">
         <v>4</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -1342,10 +1342,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="10"/>
@@ -1364,31 +1364,31 @@
         <v>6</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L10" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="L10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="M10" s="45" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>I6</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="43">
         <v>6</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1397,12 +1397,12 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="27"/>
@@ -1422,20 +1422,20 @@
         <v>6</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
+        <v>97</v>
+      </c>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" s="10">
         <v>33</v>
@@ -1453,12 +1453,12 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="11"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
@@ -1481,7 +1481,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="11"/>
       <c r="L14" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M14" s="34">
         <v>0.01</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
@@ -1512,7 +1512,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="11"/>
       <c r="L15" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M15" s="34">
         <v>1.0999999999999999E-2</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
@@ -1543,7 +1543,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="11"/>
       <c r="L16" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M16" s="34">
         <v>1.4999999999999999E-2</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
@@ -1564,7 +1564,7 @@
         <f t="shared" si="0"/>
         <v>I12</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="43">
         <v>12</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -1574,7 +1574,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="11"/>
       <c r="L17" s="33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M17" s="34">
         <v>0.02</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
@@ -1605,7 +1605,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="11"/>
       <c r="L18" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M18" s="34">
         <v>2.5000000000000001E-2</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>8</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>8</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>8</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>8</v>
@@ -1764,12 +1764,12 @@
         <v>6</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>8</v>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>8</v>
@@ -1807,7 +1807,7 @@
         <f t="shared" si="0"/>
         <v>I21</v>
       </c>
-      <c r="F26" s="46">
+      <c r="F26" s="43">
         <v>21</v>
       </c>
       <c r="G26" s="12" t="s">
@@ -1819,7 +1819,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>8</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="27"/>
@@ -1866,18 +1866,18 @@
         <v>6</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="D29" s="10">
         <v>49</v>
@@ -1954,17 +1954,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I1" s="45"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D2" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="36"/>
@@ -1979,13 +1979,13 @@
         <v>V1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J3" s="15">
         <v>2</v>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -2007,13 +2007,13 @@
         <v>V2</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4" s="15">
         <v>2</v>
@@ -2022,7 +2022,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -2035,13 +2035,13 @@
         <v>V3</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J5" s="15">
         <v>2</v>
@@ -2050,7 +2050,7 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -2063,13 +2063,13 @@
         <v>V4</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J6" s="15">
         <v>2</v>
@@ -2078,16 +2078,16 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="20"/>
       <c r="C7" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="29" t="str">
@@ -2095,7 +2095,7 @@
         <v>V5</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="38"/>
@@ -2103,16 +2103,16 @@
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="29" t="str">
@@ -2120,7 +2120,7 @@
         <v>V6</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="38"/>
@@ -2128,7 +2128,7 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -2141,13 +2141,13 @@
         <v>V7</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J9" s="15">
         <v>3</v>
@@ -2156,7 +2156,7 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -2169,13 +2169,13 @@
         <v>V8</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J10" s="15">
         <v>3</v>
@@ -2184,7 +2184,7 @@
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -2197,13 +2197,13 @@
         <v>V9</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J11" s="15">
         <v>1</v>
@@ -2212,7 +2212,7 @@
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -2225,13 +2225,13 @@
         <v>V10</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J12" s="15">
         <v>1</v>
@@ -2240,13 +2240,13 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="16"/>
       <c r="C13" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
@@ -2255,13 +2255,13 @@
         <v>V11</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J13" s="15">
         <v>1</v>
@@ -2270,16 +2270,16 @@
         <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="29" t="str">
@@ -2287,7 +2287,7 @@
         <v>V12</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="38"/>
@@ -2296,7 +2296,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -2309,13 +2309,13 @@
         <v>V13</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J15" s="15">
         <v>3</v>
@@ -2324,16 +2324,16 @@
         <v>13</v>
       </c>
       <c r="L15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="29" t="str">
@@ -2341,7 +2341,7 @@
         <v>V14</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="38"/>
@@ -2350,16 +2350,16 @@
         <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29" t="str">
@@ -2367,7 +2367,7 @@
         <v>V15</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="38"/>
@@ -2376,7 +2376,7 @@
         <v>15</v>
       </c>
       <c r="L17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
@@ -2389,13 +2389,13 @@
         <v>V16</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="35">
         <v>1</v>
@@ -2404,16 +2404,16 @@
         <v>16</v>
       </c>
       <c r="L18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="20"/>
       <c r="C19" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="29" t="str">
@@ -2421,7 +2421,7 @@
         <v>V17</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="38"/>
@@ -2430,16 +2430,16 @@
         <v>17</v>
       </c>
       <c r="L19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="29" t="str">
@@ -2447,7 +2447,7 @@
         <v>V18</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="38"/>
@@ -2456,7 +2456,7 @@
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J21" s="15">
         <v>3</v>
@@ -2484,7 +2484,7 @@
         <v>19</v>
       </c>
       <c r="L21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -2497,13 +2497,13 @@
         <v>V20</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I22" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J22" s="15">
         <v>3</v>
@@ -2512,16 +2512,16 @@
         <v>20</v>
       </c>
       <c r="L22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="29" t="str">
@@ -2529,7 +2529,7 @@
         <v>V21</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="36"/>
@@ -2537,16 +2537,16 @@
         <v>21</v>
       </c>
       <c r="L23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="20"/>
       <c r="C24" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E24" s="30">
         <v>42</v>
@@ -2556,7 +2556,7 @@
         <v>V22</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="36"/>
@@ -2564,16 +2564,16 @@
         <v>22</v>
       </c>
       <c r="L24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="23"/>
       <c r="C25" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E25" s="31"/>
       <c r="F25" s="29" t="str">
@@ -2581,7 +2581,7 @@
         <v>V23</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="36"/>
@@ -2589,7 +2589,7 @@
         <v>23</v>
       </c>
       <c r="L25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>V24</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="36"/>
@@ -2614,7 +2614,7 @@
         <v>24</v>
       </c>
       <c r="L26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>V25</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="36"/>
@@ -2639,7 +2639,7 @@
         <v>25</v>
       </c>
       <c r="L27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>V26</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="36"/>
@@ -2664,7 +2664,7 @@
         <v>26</v>
       </c>
       <c r="L28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>V27</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="36"/>
@@ -2689,7 +2689,7 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>V28</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="36"/>
@@ -2714,7 +2714,7 @@
         <v>28</v>
       </c>
       <c r="L30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
@@ -2731,7 +2731,7 @@
         <v>V29</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="36"/>
@@ -2739,7 +2739,7 @@
         <v>29</v>
       </c>
       <c r="L31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
         <v>V30</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="36"/>
@@ -2764,7 +2764,7 @@
         <v>30</v>
       </c>
       <c r="L32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2789,7 +2789,7 @@
         <v>31</v>
       </c>
       <c r="L33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
@@ -2814,13 +2814,13 @@
         <v>32</v>
       </c>
       <c r="L34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="20"/>
       <c r="C35" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30">
@@ -2839,13 +2839,13 @@
         <v>33</v>
       </c>
       <c r="L35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="23"/>
       <c r="C36" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="31"/>
       <c r="E36" s="31">
@@ -2856,7 +2856,7 @@
         <v>V34</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H36" s="25"/>
       <c r="I36" s="36"/>
@@ -2864,7 +2864,7 @@
         <v>34</v>
       </c>
       <c r="L36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -2885,7 +2885,7 @@
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E39"/>
       <c r="F39"/>
@@ -2894,7 +2894,7 @@
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E40"/>
       <c r="F40"/>
@@ -2909,7 +2909,7 @@
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42"/>
       <c r="C42" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -2929,7 +2929,7 @@
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44"/>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D44">
         <v>10</v>
@@ -3318,22 +3318,22 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>